<commit_message>
change Pacman class, store 1000 rounds points.
</commit_message>
<xml_diff>
--- a/Pacman.xlsx
+++ b/Pacman.xlsx
@@ -652,7 +652,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,9 +1037,6 @@
       <c r="M12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P12">
-        <v>11</v>
-      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M13" s="1" t="s">
@@ -1048,9 +1045,6 @@
       <c r="N13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P13">
-        <v>110</v>
-      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M14" s="7" t="s">
@@ -1059,9 +1053,6 @@
       <c r="N14" s="8">
         <v>0</v>
       </c>
-      <c r="P14">
-        <v>101</v>
-      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="M15" s="7" t="s">
@@ -1069,9 +1060,6 @@
       </c>
       <c r="N15" s="8">
         <v>10</v>
-      </c>
-      <c r="P15">
-        <v>1010</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add test checker to document.
</commit_message>
<xml_diff>
--- a/Pacman.xlsx
+++ b/Pacman.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzhanjud\Documents\GitHub\Pacman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdkjizh941\Documents\Judy\Pacman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
   <si>
     <t>↑</t>
   </si>
@@ -86,9 +86,6 @@
     <t>GAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>MOVE NUMBER/ROUND</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>200 MOVES/ROUND</t>
+  </si>
+  <si>
+    <t>●</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -307,11 +307,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,6 +409,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,16 +698,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="2" max="3" width="3.28515625" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
@@ -756,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T2" s="20">
         <v>1000</v>
@@ -795,7 +843,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T3" s="8">
         <v>200</v>
@@ -828,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T4" s="8">
         <v>200</v>
@@ -867,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T5" s="8">
         <v>50</v>
@@ -911,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1055,6 +1103,27 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="23"/>
       <c r="M15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1063,6 +1132,29 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="26"/>
       <c r="M16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1070,7 +1162,28 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="M17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1078,9 +1191,183 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J20" t="s">
-        <v>20</v>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="28"/>
+      <c r="K24" s="29" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add run game unit test
</commit_message>
<xml_diff>
--- a/Pacman.xlsx
+++ b/Pacman.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="270">
   <si>
     <t>↑</t>
   </si>
@@ -102,6 +102,738 @@
   </si>
   <si>
     <t>●</t>
+  </si>
+  <si>
+    <t>Strategy:</t>
+  </si>
+  <si>
+    <t>Key: 00000 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 00001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00002 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 00011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00012 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 00020 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 00021 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00022 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00100 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 00101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00102 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00110 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 00111 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00112 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00120 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 00121 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00122 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00200 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00202 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00210 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00211 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00212 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00220 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 00221 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 00222 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01000 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 01001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 01002 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01010 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 01012 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01020 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 01021 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01022 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 01100 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 01102 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01110 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01111 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01112 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01120 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01121 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01122 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 01200 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 01202 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01210 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 01211 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01212 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01220 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 01221 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 01222 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 02000 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 02001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02002 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 02011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02012 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02020 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02021 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02022 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02100 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 02101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02102 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02110 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 02111 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02112 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02120 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 02121 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 02122 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 02200 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 02201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02202 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 02210 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 02211 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02212 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02220 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 02221 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 02222 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10000 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 10001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10002 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10010 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 10011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10012 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10020 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10021 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10022 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10100 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10102 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 10110 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10111 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10112 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 10120 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10121 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10122 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 10200 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 10201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10202 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 10210 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 10211 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 10212 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 10220 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 10221 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 10222 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 11000 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 11002 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 11010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11011 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11012 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11020 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 11021 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 11022 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11100 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11101 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11102 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11110 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11111 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11112 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11120 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 11121 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 11122 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11200 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11201 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11202 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 11210 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11211 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11212 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11220 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 11221 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 11222 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12000 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 12001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12002 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 12011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12012 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12020 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 12021 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12022 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 12100 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 12101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12102 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12110 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12111 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12112 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 12120 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12121 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12122 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12200 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 12201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12202 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12210 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 12211 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12212 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 12220 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 12221 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 12222 Value:up</t>
+  </si>
+  <si>
+    <t>Key: 20000 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 20001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20002 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 20011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20012 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20020 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 20021 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20022 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 20100 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 20101 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20102 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20110 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20111 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20112 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20120 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 20121 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20122 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 20200 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 20201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20202 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 20210 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20211 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 20212 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20220 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20221 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 20222 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21000 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 21001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 21002 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 21010 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21011 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21012 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21020 Value:right</t>
+  </si>
+  <si>
+    <t>Key: 21021 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21022 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 21100 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21101 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21102 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21110 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21111 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 21112 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 21120 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21121 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 21122 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 21200 Value:freeze</t>
+  </si>
+  <si>
+    <t>Key: 21201 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21202 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21210 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21211 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21212 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21220 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21221 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 21222 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22000 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 22001 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 22002 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22010 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 22011 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 22012 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 22020 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22021 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22022 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 22100 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22101 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22102 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22110 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22111 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22112 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22120 Value:down</t>
+  </si>
+  <si>
+    <t>Key: 22121 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22122 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22200 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22201 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 22202 Value:left</t>
+  </si>
+  <si>
+    <t>Key: 22210 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22211 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22212 Value:eat</t>
+  </si>
+  <si>
+    <t>Key: 22220 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22221 Value:random</t>
+  </si>
+  <si>
+    <t>Key: 22222 Value:random</t>
   </si>
 </sst>
 </file>
@@ -698,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:V245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,9 +1452,10 @@
     <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3">
         <v>1</v>
       </c>
@@ -762,8 +1495,11 @@
       <c r="S1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -810,7 +1546,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -848,8 +1584,11 @@
       <c r="T3" s="8">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -881,8 +1620,11 @@
       <c r="T4" s="8">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -920,8 +1662,11 @@
       <c r="T5" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -961,8 +1706,11 @@
       <c r="T6" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -988,8 +1736,11 @@
       <c r="N7" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1009,8 +1760,11 @@
       <c r="N8" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1030,8 +1784,11 @@
       <c r="N9" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1051,8 +1808,11 @@
       <c r="K10" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1080,29 +1840,41 @@
       <c r="K11" s="18">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M12" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="N14" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1130,8 +1902,11 @@
       <c r="N15" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1161,8 +1936,11 @@
       <c r="N16" s="8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1190,8 +1968,11 @@
       <c r="N17" s="10">
         <v>-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1213,8 +1994,11 @@
       <c r="K18" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1236,8 +2020,11 @@
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="26"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1261,8 +2048,11 @@
         <v>25</v>
       </c>
       <c r="K20" s="26"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1288,8 +2078,11 @@
       <c r="K21" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1317,8 +2110,11 @@
       <c r="K22" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1346,8 +2142,11 @@
         <v>25</v>
       </c>
       <c r="K23" s="26"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1368,6 +2167,1114 @@
       <c r="J24" s="28"/>
       <c r="K24" s="29" t="s">
         <v>25</v>
+      </c>
+      <c r="V24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V63" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V70" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V72" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V78" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V79" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V80" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V83" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V84" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V87" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V88" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V89" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V91" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V92" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V93" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V94" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V95" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="96" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V96" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V97" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="98" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V98" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="99" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V101" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V102" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="103" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V103" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V104" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="105" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V105" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="106" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V106" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V107" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V108" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="109" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V109" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="110" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V110" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="111" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V111" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V112" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="113" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V113" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="114" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V114" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V115" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="116" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V116" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V117" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="118" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V118" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V119" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="120" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V120" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V121" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="122" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V122" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="123" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V123" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="124" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V124" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="125" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V125" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="126" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V126" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V127" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="128" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V128" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="129" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V129" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="130" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V130" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="131" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V131" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="132" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V132" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="133" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V133" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="134" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V134" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="135" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V135" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="136" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V136" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="137" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V137" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="138" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V138" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="139" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V139" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="140" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V140" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="141" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V141" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="142" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V142" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="143" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V143" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="144" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V144" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="145" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V145" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="146" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V146" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="147" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V147" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="148" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V148" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="149" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V149" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="150" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V150" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="151" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V151" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="152" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V152" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="153" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V153" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="154" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V154" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="155" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V155" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="156" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V156" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="157" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V157" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="158" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V158" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="159" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V159" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="160" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V160" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="161" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V161" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="162" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V162" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="163" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V163" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="164" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V164" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="165" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V165" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="166" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V166" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="167" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V167" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="168" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V168" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="169" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V169" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="170" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V170" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="171" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V171" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="172" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V172" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="173" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V173" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="174" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V174" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="175" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V175" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="176" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V176" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="177" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V177" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="178" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V178" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="179" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V179" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="180" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V180" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="181" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V181" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="182" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V182" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="183" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V183" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="184" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V184" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="185" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V185" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V186" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="187" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V187" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="188" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V188" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="189" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V189" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="190" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V190" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="191" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V191" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="192" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V192" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="193" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V193" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="194" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V194" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="195" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V195" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="196" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V196" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="197" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V197" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="198" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V198" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="199" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V199" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="200" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V200" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="201" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V201" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="202" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V202" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="203" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V203" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="204" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V204" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="205" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V205" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="206" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V206" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="207" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V207" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="208" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V208" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="209" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V209" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="210" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V210" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="211" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V211" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="212" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V212" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="213" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V213" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="214" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V214" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="215" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V215" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="216" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V216" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="217" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V217" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="218" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V218" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="219" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V219" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="220" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V220" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="221" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V221" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="222" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V222" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="223" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V223" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="224" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V224" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="225" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V225" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="226" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V226" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="227" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V227" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="228" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V228" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="229" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V229" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="230" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V230" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="231" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V231" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="232" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V232" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="233" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V233" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="234" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V234" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="235" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V235" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="236" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V236" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="237" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V237" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="238" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V238" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="239" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V239" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="240" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V240" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="241" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V241" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="242" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V242" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="243" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V243" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="244" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V244" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="245" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V245" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>